<commit_message>
much better, more prop_keys founded
</commit_message>
<xml_diff>
--- a/Data_Dictionary/xlsx/Columns/Proponentes_columns.xlsx
+++ b/Data_Dictionary/xlsx/Columns/Proponentes_columns.xlsx
@@ -14,12 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>columns</t>
   </si>
   <si>
     <t>descricao</t>
+  </si>
+  <si>
+    <t>Unnamed: 0</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1</t>
   </si>
   <si>
     <t>prop_pk1</t>
@@ -404,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -490,6 +499,30 @@
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>